<commit_message>
working on opening page - finished header
</commit_message>
<xml_diff>
--- a/snakeHeader.xlsx
+++ b/snakeHeader.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Leah London Arazi\Dropbox\My PC (Leah-X1-Carbon)\Documents\Leah X1 Carbon\university\2022a\web\snake\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC668814-10DC-4E9C-A5A1-C2975FE41C9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7230892-A557-4B48-BB73-E7D4423D1BCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19310" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{ECD35F3C-53EF-403A-A9C4-9637056E55AE}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{ECD35F3C-53EF-403A-A9C4-9637056E55AE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,10 +35,6 @@
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
@@ -50,7 +46,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -93,6 +89,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7030A0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -121,7 +129,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -133,6 +141,8 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3064,13 +3074,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B56EF5FC-152E-468A-8987-1B0BC1265AB3}">
   <dimension ref="A1:AX50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AL30" sqref="AL30"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.42578125" customWidth="1"/>
     <col min="50" max="50" width="3.42578125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3080,7 +3090,7 @@
         <v>[0,0]</v>
       </c>
       <c r="B1" s="1" t="str">
-        <f t="shared" ref="B1:AX6" si="0">_xlfn.CONCAT("[",ROW(B1)-1,",",COLUMN(B1)-1,"]")</f>
+        <f t="shared" ref="B1:AX1" si="0">_xlfn.CONCAT("[",ROW(B1)-1,",",COLUMN(B1)-1,"]")</f>
         <v>[0,1]</v>
       </c>
       <c r="C1" s="1" t="str">
@@ -3278,7 +3288,7 @@
     </row>
     <row r="2" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="str">
-        <f t="shared" ref="A2:P33" si="1">_xlfn.CONCAT("[",ROW(A2)-1,",",COLUMN(A2)-1,"]")</f>
+        <f t="shared" ref="A2:P17" si="1">_xlfn.CONCAT("[",ROW(A2)-1,",",COLUMN(A2)-1,"]")</f>
         <v>[1,0]</v>
       </c>
       <c r="B2" s="1" t="str">
@@ -3342,7 +3352,7 @@
         <v>[1,15]</v>
       </c>
       <c r="Q2" s="1" t="str">
-        <f t="shared" ref="Q2:AF50" si="2">_xlfn.CONCAT("[",ROW(Q2)-1,",",COLUMN(Q2)-1,"]")</f>
+        <f t="shared" ref="Q2:AF31" si="2">_xlfn.CONCAT("[",ROW(Q2)-1,",",COLUMN(Q2)-1,"]")</f>
         <v>[1,16]</v>
       </c>
       <c r="R2" s="1" t="str">
@@ -3406,7 +3416,7 @@
         <v>[1,31]</v>
       </c>
       <c r="AG2" s="1" t="str">
-        <f t="shared" ref="AG2:AV50" si="3">_xlfn.CONCAT("[",ROW(AG2)-1,",",COLUMN(AG2)-1,"]")</f>
+        <f t="shared" ref="AG2:AV17" si="3">_xlfn.CONCAT("[",ROW(AG2)-1,",",COLUMN(AG2)-1,"]")</f>
         <v>[1,32]</v>
       </c>
       <c r="AH2" s="1" t="str">
@@ -3470,7 +3480,7 @@
         <v>[1,47]</v>
       </c>
       <c r="AW2" s="1" t="str">
-        <f t="shared" ref="AW2:AX50" si="4">_xlfn.CONCAT("[",ROW(AW2)-1,",",COLUMN(AW2)-1,"]")</f>
+        <f t="shared" ref="AW2:AX16" si="4">_xlfn.CONCAT("[",ROW(AW2)-1,",",COLUMN(AW2)-1,"]")</f>
         <v>[1,48]</v>
       </c>
       <c r="AX2" s="1" t="str">
@@ -6368,7 +6378,7 @@
         <v>[16,14]</v>
       </c>
       <c r="P17" s="1" t="str">
-        <f t="shared" ref="P17:AE50" si="5">_xlfn.CONCAT("[",ROW(P17)-1,",",COLUMN(P17)-1,"]")</f>
+        <f t="shared" ref="P17:AE32" si="5">_xlfn.CONCAT("[",ROW(P17)-1,",",COLUMN(P17)-1,"]")</f>
         <v>[16,15]</v>
       </c>
       <c r="Q17" s="1" t="str">
@@ -6496,7 +6506,7 @@
         <v>[16,46]</v>
       </c>
       <c r="AV17" s="1" t="str">
-        <f t="shared" ref="AV17:AX50" si="6">_xlfn.CONCAT("[",ROW(AV17)-1,",",COLUMN(AV17)-1,"]")</f>
+        <f t="shared" ref="AV17:AX46" si="6">_xlfn.CONCAT("[",ROW(AV17)-1,",",COLUMN(AV17)-1,"]")</f>
         <v>[16,47]</v>
       </c>
       <c r="AW17" s="1" t="str">
@@ -6510,7 +6520,7 @@
     </row>
     <row r="18" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="str">
-        <f t="shared" ref="A18:P50" si="7">_xlfn.CONCAT("[",ROW(A18)-1,",",COLUMN(A18)-1,"]")</f>
+        <f t="shared" ref="A18:P33" si="7">_xlfn.CONCAT("[",ROW(A18)-1,",",COLUMN(A18)-1,"]")</f>
         <v>[17,0]</v>
       </c>
       <c r="B18" s="1" t="str">
@@ -6638,7 +6648,7 @@
         <v>[17,31]</v>
       </c>
       <c r="AG18" s="1" t="str">
-        <f t="shared" ref="AG18:AV50" si="8">_xlfn.CONCAT("[",ROW(AG18)-1,",",COLUMN(AG18)-1,"]")</f>
+        <f t="shared" ref="AG18:AV46" si="8">_xlfn.CONCAT("[",ROW(AG18)-1,",",COLUMN(AG18)-1,"]")</f>
         <v>[17,32]</v>
       </c>
       <c r="AH18" s="1" t="str">
@@ -6799,27 +6809,27 @@
         <f t="shared" si="5"/>
         <v>[18,21]</v>
       </c>
-      <c r="W19" s="3" t="str">
+      <c r="W19" s="4" t="str">
         <f t="shared" si="5"/>
         <v>[18,22]</v>
       </c>
-      <c r="X19" s="3" t="str">
+      <c r="X19" s="4" t="str">
         <f t="shared" si="5"/>
         <v>[18,23]</v>
       </c>
-      <c r="Y19" s="3" t="str">
+      <c r="Y19" s="4" t="str">
         <f t="shared" si="5"/>
         <v>[18,24]</v>
       </c>
-      <c r="Z19" s="3" t="str">
+      <c r="Z19" s="4" t="str">
         <f t="shared" si="5"/>
         <v>[18,25]</v>
       </c>
-      <c r="AA19" s="3" t="str">
+      <c r="AA19" s="4" t="str">
         <f t="shared" si="5"/>
         <v>[18,26]</v>
       </c>
-      <c r="AB19" s="3" t="str">
+      <c r="AB19" s="4" t="str">
         <f t="shared" si="5"/>
         <v>[18,27]</v>
       </c>
@@ -6831,7 +6841,7 @@
         <f t="shared" si="5"/>
         <v>[18,29]</v>
       </c>
-      <c r="AE19" s="3" t="str">
+      <c r="AE19" s="4" t="str">
         <f t="shared" si="5"/>
         <v>[18,30]</v>
       </c>
@@ -6855,7 +6865,7 @@
         <f t="shared" si="8"/>
         <v>[18,35]</v>
       </c>
-      <c r="AK19" s="3" t="str">
+      <c r="AK19" s="4" t="str">
         <f t="shared" si="8"/>
         <v>[18,36]</v>
       </c>
@@ -6875,24 +6885,24 @@
         <f t="shared" si="8"/>
         <v>[18,40]</v>
       </c>
-      <c r="AP19" s="3" t="str">
+      <c r="AP19" s="11" t="str">
         <f t="shared" si="8"/>
         <v>[18,41]</v>
       </c>
-      <c r="AQ19" s="3" t="str">
+      <c r="AQ19" s="4" t="str">
         <f t="shared" si="8"/>
         <v>[18,42]</v>
       </c>
-      <c r="AR19" s="3" t="str">
+      <c r="AR19" s="11" t="str">
         <f t="shared" si="8"/>
         <v>[18,43]</v>
       </c>
-      <c r="AS19" s="3" t="str">
+      <c r="AS19" s="7" t="str">
         <f t="shared" si="8"/>
         <v>[18,44]</v>
       </c>
-      <c r="AT19" s="3" t="str">
-        <f t="shared" si="8"/>
+      <c r="AT19" s="4" t="str">
+        <f>_xlfn.CONCAT("[",ROW(AT19)-1,",",COLUMN(AT19)-1,"]")</f>
         <v>[18,45]</v>
       </c>
       <c r="AU19" s="1" t="str">
@@ -7001,7 +7011,7 @@
         <f t="shared" si="5"/>
         <v>[19,21]</v>
       </c>
-      <c r="W20" s="3" t="str">
+      <c r="W20" s="4" t="str">
         <f t="shared" si="5"/>
         <v>[19,22]</v>
       </c>
@@ -7021,7 +7031,7 @@
         <f t="shared" si="5"/>
         <v>[19,26]</v>
       </c>
-      <c r="AB20" s="3" t="str">
+      <c r="AB20" s="4" t="str">
         <f t="shared" si="5"/>
         <v>[19,27]</v>
       </c>
@@ -7033,7 +7043,7 @@
         <f t="shared" si="5"/>
         <v>[19,29]</v>
       </c>
-      <c r="AE20" s="3" t="str">
+      <c r="AE20" s="4" t="str">
         <f t="shared" si="5"/>
         <v>[19,30]</v>
       </c>
@@ -7057,7 +7067,7 @@
         <f t="shared" si="8"/>
         <v>[19,35]</v>
       </c>
-      <c r="AK20" s="3" t="str">
+      <c r="AK20" s="4" t="str">
         <f t="shared" si="8"/>
         <v>[19,36]</v>
       </c>
@@ -7203,7 +7213,7 @@
         <f t="shared" si="5"/>
         <v>[20,21]</v>
       </c>
-      <c r="W21" s="3" t="str">
+      <c r="W21" s="4" t="str">
         <f t="shared" si="5"/>
         <v>[20,22]</v>
       </c>
@@ -7223,7 +7233,7 @@
         <f t="shared" si="5"/>
         <v>[20,26]</v>
       </c>
-      <c r="AB21" s="3" t="str">
+      <c r="AB21" s="4" t="str">
         <f t="shared" si="5"/>
         <v>[20,27]</v>
       </c>
@@ -7235,7 +7245,7 @@
         <f t="shared" si="5"/>
         <v>[20,29]</v>
       </c>
-      <c r="AE21" s="3" t="str">
+      <c r="AE21" s="11" t="str">
         <f t="shared" si="5"/>
         <v>[20,30]</v>
       </c>
@@ -7251,15 +7261,15 @@
         <f t="shared" si="8"/>
         <v>[20,33]</v>
       </c>
-      <c r="AI21" s="3" t="str">
+      <c r="AI21" s="12" t="str">
         <f t="shared" si="8"/>
         <v>[20,34]</v>
       </c>
-      <c r="AJ21" s="3" t="str">
+      <c r="AJ21" s="7" t="str">
         <f t="shared" si="8"/>
         <v>[20,35]</v>
       </c>
-      <c r="AK21" s="3" t="str">
+      <c r="AK21" s="11" t="str">
         <f t="shared" si="8"/>
         <v>[20,36]</v>
       </c>
@@ -7271,7 +7281,7 @@
         <f t="shared" si="8"/>
         <v>[20,38]</v>
       </c>
-      <c r="AN21" s="3" t="str">
+      <c r="AN21" s="11" t="str">
         <f t="shared" si="8"/>
         <v>[20,39]</v>
       </c>
@@ -7405,7 +7415,7 @@
         <f t="shared" si="5"/>
         <v>[21,21]</v>
       </c>
-      <c r="W22" s="3" t="str">
+      <c r="W22" s="4" t="str">
         <f t="shared" si="5"/>
         <v>[21,22]</v>
       </c>
@@ -7425,7 +7435,7 @@
         <f t="shared" si="5"/>
         <v>[21,26]</v>
       </c>
-      <c r="AB22" s="3" t="str">
+      <c r="AB22" s="4" t="str">
         <f t="shared" si="5"/>
         <v>[21,27]</v>
       </c>
@@ -7437,7 +7447,7 @@
         <f t="shared" si="5"/>
         <v>[21,29]</v>
       </c>
-      <c r="AE22" s="3" t="str">
+      <c r="AE22" s="7" t="str">
         <f t="shared" si="5"/>
         <v>[21,30]</v>
       </c>
@@ -7473,7 +7483,7 @@
         <f t="shared" si="8"/>
         <v>[21,38]</v>
       </c>
-      <c r="AN22" s="3" t="str">
+      <c r="AN22" s="4" t="str">
         <f t="shared" si="8"/>
         <v>[21,39]</v>
       </c>
@@ -7607,7 +7617,7 @@
         <f t="shared" si="5"/>
         <v>[22,21]</v>
       </c>
-      <c r="W23" s="3" t="str">
+      <c r="W23" s="4" t="str">
         <f t="shared" si="5"/>
         <v>[22,22]</v>
       </c>
@@ -7627,7 +7637,7 @@
         <f t="shared" si="5"/>
         <v>[22,26]</v>
       </c>
-      <c r="AB23" s="3" t="str">
+      <c r="AB23" s="4" t="str">
         <f t="shared" si="5"/>
         <v>[22,27]</v>
       </c>
@@ -7639,7 +7649,7 @@
         <f t="shared" si="5"/>
         <v>[22,29]</v>
       </c>
-      <c r="AE23" s="3" t="str">
+      <c r="AE23" s="12" t="str">
         <f t="shared" si="5"/>
         <v>[22,30]</v>
       </c>
@@ -7647,11 +7657,11 @@
         <f t="shared" si="2"/>
         <v>[22,31]</v>
       </c>
-      <c r="AG23" s="3" t="str">
+      <c r="AG23" s="7" t="str">
         <f t="shared" si="8"/>
         <v>[22,32]</v>
       </c>
-      <c r="AH23" s="3" t="str">
+      <c r="AH23" s="12" t="str">
         <f t="shared" si="8"/>
         <v>[22,33]</v>
       </c>
@@ -7675,7 +7685,7 @@
         <f t="shared" si="8"/>
         <v>[22,38]</v>
       </c>
-      <c r="AN23" s="3" t="str">
+      <c r="AN23" s="11" t="str">
         <f t="shared" si="8"/>
         <v>[22,39]</v>
       </c>
@@ -7809,7 +7819,7 @@
         <f t="shared" si="5"/>
         <v>[23,21]</v>
       </c>
-      <c r="W24" s="3" t="str">
+      <c r="W24" s="4" t="str">
         <f t="shared" si="5"/>
         <v>[23,22]</v>
       </c>
@@ -7829,7 +7839,7 @@
         <f t="shared" si="5"/>
         <v>[23,26]</v>
       </c>
-      <c r="AB24" s="3" t="str">
+      <c r="AB24" s="4" t="str">
         <f t="shared" si="5"/>
         <v>[23,27]</v>
       </c>
@@ -7849,7 +7859,7 @@
         <f t="shared" si="2"/>
         <v>[23,31]</v>
       </c>
-      <c r="AG24" s="3" t="str">
+      <c r="AG24" s="11" t="str">
         <f t="shared" si="8"/>
         <v>[23,32]</v>
       </c>
@@ -7877,7 +7887,7 @@
         <f t="shared" si="8"/>
         <v>[23,38]</v>
       </c>
-      <c r="AN24" s="3" t="str">
+      <c r="AN24" s="11" t="str">
         <f t="shared" si="8"/>
         <v>[23,39]</v>
       </c>
@@ -8047,11 +8057,11 @@
         <f t="shared" si="5"/>
         <v>[24,30]</v>
       </c>
-      <c r="AF25" s="3" t="str">
+      <c r="AF25" s="4" t="str">
         <f t="shared" si="2"/>
         <v>[24,31]</v>
       </c>
-      <c r="AG25" s="3" t="str">
+      <c r="AG25" s="4" t="str">
         <f t="shared" si="8"/>
         <v>[24,32]</v>
       </c>
@@ -8083,27 +8093,27 @@
         <f t="shared" si="8"/>
         <v>[24,39]</v>
       </c>
-      <c r="AO25" s="3" t="str">
+      <c r="AO25" s="11" t="str">
         <f t="shared" si="8"/>
         <v>[24,40]</v>
       </c>
-      <c r="AP25" s="3" t="str">
+      <c r="AP25" s="11" t="str">
         <f t="shared" si="8"/>
         <v>[24,41]</v>
       </c>
-      <c r="AQ25" s="3" t="str">
+      <c r="AQ25" s="4" t="str">
         <f t="shared" si="8"/>
         <v>[24,42]</v>
       </c>
-      <c r="AR25" s="3" t="str">
+      <c r="AR25" s="11" t="str">
         <f t="shared" si="8"/>
         <v>[24,43]</v>
       </c>
-      <c r="AS25" s="3" t="str">
+      <c r="AS25" s="7" t="str">
         <f t="shared" si="8"/>
         <v>[24,44]</v>
       </c>
-      <c r="AT25" s="3" t="str">
+      <c r="AT25" s="4" t="str">
         <f t="shared" si="8"/>
         <v>[24,45]</v>
       </c>
@@ -8249,11 +8259,11 @@
         <f t="shared" si="5"/>
         <v>[25,30]</v>
       </c>
-      <c r="AF26" s="3" t="str">
+      <c r="AF26" s="4" t="str">
         <f t="shared" si="2"/>
         <v>[25,31]</v>
       </c>
-      <c r="AG26" s="3" t="str">
+      <c r="AG26" s="11" t="str">
         <f t="shared" si="8"/>
         <v>[25,32]</v>
       </c>
@@ -8415,7 +8425,7 @@
         <f t="shared" si="5"/>
         <v>[26,21]</v>
       </c>
-      <c r="W27" s="3" t="str">
+      <c r="W27" s="4" t="str">
         <f t="shared" si="5"/>
         <v>[26,22]</v>
       </c>
@@ -8435,7 +8445,7 @@
         <f t="shared" si="5"/>
         <v>[26,26]</v>
       </c>
-      <c r="AB27" s="3" t="str">
+      <c r="AB27" s="4" t="str">
         <f t="shared" si="5"/>
         <v>[26,27]</v>
       </c>
@@ -8455,7 +8465,7 @@
         <f t="shared" si="2"/>
         <v>[26,31]</v>
       </c>
-      <c r="AG27" s="3" t="str">
+      <c r="AG27" s="11" t="str">
         <f t="shared" si="8"/>
         <v>[26,32]</v>
       </c>
@@ -8483,7 +8493,7 @@
         <f t="shared" si="8"/>
         <v>[26,38]</v>
       </c>
-      <c r="AN27" s="3" t="str">
+      <c r="AN27" s="11" t="str">
         <f t="shared" si="8"/>
         <v>[26,39]</v>
       </c>
@@ -8617,7 +8627,7 @@
         <f t="shared" si="5"/>
         <v>[27,21]</v>
       </c>
-      <c r="W28" s="3" t="str">
+      <c r="W28" s="4" t="str">
         <f t="shared" si="5"/>
         <v>[27,22]</v>
       </c>
@@ -8637,7 +8647,7 @@
         <f t="shared" si="5"/>
         <v>[27,26]</v>
       </c>
-      <c r="AB28" s="3" t="str">
+      <c r="AB28" s="4" t="str">
         <f t="shared" si="5"/>
         <v>[27,27]</v>
       </c>
@@ -8649,7 +8659,7 @@
         <f t="shared" si="5"/>
         <v>[27,29]</v>
       </c>
-      <c r="AE28" s="3" t="str">
+      <c r="AE28" s="12" t="str">
         <f t="shared" si="5"/>
         <v>[27,30]</v>
       </c>
@@ -8657,11 +8667,11 @@
         <f t="shared" si="2"/>
         <v>[27,31]</v>
       </c>
-      <c r="AG28" s="3" t="str">
+      <c r="AG28" s="7" t="str">
         <f t="shared" si="8"/>
         <v>[27,32]</v>
       </c>
-      <c r="AH28" s="3" t="str">
+      <c r="AH28" s="12" t="str">
         <f t="shared" si="8"/>
         <v>[27,33]</v>
       </c>
@@ -8685,7 +8695,7 @@
         <f t="shared" si="8"/>
         <v>[27,38]</v>
       </c>
-      <c r="AN28" s="3" t="str">
+      <c r="AN28" s="11" t="str">
         <f t="shared" si="8"/>
         <v>[27,39]</v>
       </c>
@@ -8819,7 +8829,7 @@
         <f t="shared" si="5"/>
         <v>[28,21]</v>
       </c>
-      <c r="W29" s="3" t="str">
+      <c r="W29" s="4" t="str">
         <f t="shared" si="5"/>
         <v>[28,22]</v>
       </c>
@@ -8839,7 +8849,7 @@
         <f t="shared" si="5"/>
         <v>[28,26]</v>
       </c>
-      <c r="AB29" s="3" t="str">
+      <c r="AB29" s="4" t="str">
         <f t="shared" si="5"/>
         <v>[28,27]</v>
       </c>
@@ -8851,7 +8861,7 @@
         <f t="shared" si="5"/>
         <v>[28,29]</v>
       </c>
-      <c r="AE29" s="3" t="str">
+      <c r="AE29" s="7" t="str">
         <f t="shared" si="5"/>
         <v>[28,30]</v>
       </c>
@@ -8887,7 +8897,7 @@
         <f t="shared" si="8"/>
         <v>[28,38]</v>
       </c>
-      <c r="AN29" s="3" t="str">
+      <c r="AN29" s="4" t="str">
         <f t="shared" si="8"/>
         <v>[28,39]</v>
       </c>
@@ -9021,7 +9031,7 @@
         <f t="shared" si="5"/>
         <v>[29,21]</v>
       </c>
-      <c r="W30" s="3" t="str">
+      <c r="W30" s="4" t="str">
         <f t="shared" si="5"/>
         <v>[29,22]</v>
       </c>
@@ -9041,7 +9051,7 @@
         <f t="shared" si="5"/>
         <v>[29,26]</v>
       </c>
-      <c r="AB30" s="3" t="str">
+      <c r="AB30" s="4" t="str">
         <f t="shared" si="5"/>
         <v>[29,27]</v>
       </c>
@@ -9053,7 +9063,7 @@
         <f t="shared" si="5"/>
         <v>[29,29]</v>
       </c>
-      <c r="AE30" s="3" t="str">
+      <c r="AE30" s="11" t="str">
         <f t="shared" si="5"/>
         <v>[29,30]</v>
       </c>
@@ -9069,15 +9079,15 @@
         <f t="shared" si="8"/>
         <v>[29,33]</v>
       </c>
-      <c r="AI30" s="3" t="str">
+      <c r="AI30" s="12" t="str">
         <f t="shared" si="8"/>
         <v>[29,34]</v>
       </c>
-      <c r="AJ30" s="3" t="str">
+      <c r="AJ30" s="7" t="str">
         <f t="shared" si="8"/>
         <v>[29,35]</v>
       </c>
-      <c r="AK30" s="3" t="str">
+      <c r="AK30" s="11" t="str">
         <f t="shared" si="8"/>
         <v>[29,36]</v>
       </c>
@@ -9089,7 +9099,7 @@
         <f t="shared" si="8"/>
         <v>[29,38]</v>
       </c>
-      <c r="AN30" s="3" t="str">
+      <c r="AN30" s="11" t="str">
         <f t="shared" si="8"/>
         <v>[29,39]</v>
       </c>
@@ -9462,7 +9472,7 @@
         <v>[31,30]</v>
       </c>
       <c r="AF32" s="1" t="str">
-        <f t="shared" ref="AF32:AU50" si="9">_xlfn.CONCAT("[",ROW(AF32)-1,",",COLUMN(AF32)-1,"]")</f>
+        <f t="shared" ref="AF32:AU47" si="9">_xlfn.CONCAT("[",ROW(AF32)-1,",",COLUMN(AF32)-1,"]")</f>
         <v>[31,31]</v>
       </c>
       <c r="AG32" s="1" t="str">
@@ -9501,23 +9511,23 @@
         <f t="shared" si="9"/>
         <v>[31,40]</v>
       </c>
-      <c r="AP32" s="3" t="str">
+      <c r="AP32" s="11" t="str">
         <f t="shared" si="9"/>
         <v>[31,41]</v>
       </c>
-      <c r="AQ32" s="3" t="str">
+      <c r="AQ32" s="4" t="str">
         <f t="shared" si="9"/>
         <v>[31,42]</v>
       </c>
-      <c r="AR32" s="3" t="str">
+      <c r="AR32" s="11" t="str">
         <f t="shared" si="9"/>
         <v>[31,43]</v>
       </c>
-      <c r="AS32" s="3" t="str">
+      <c r="AS32" s="7" t="str">
         <f t="shared" si="9"/>
         <v>[31,44]</v>
       </c>
-      <c r="AT32" s="3" t="str">
+      <c r="AT32" s="4" t="str">
         <f t="shared" si="9"/>
         <v>[31,45]</v>
       </c>
@@ -9600,7 +9610,7 @@
         <v>[32,14]</v>
       </c>
       <c r="P33" s="1" t="str">
-        <f t="shared" ref="P33:AE50" si="10">_xlfn.CONCAT("[",ROW(P33)-1,",",COLUMN(P33)-1,"]")</f>
+        <f t="shared" ref="P33:AE48" si="10">_xlfn.CONCAT("[",ROW(P33)-1,",",COLUMN(P33)-1,"]")</f>
         <v>[32,15]</v>
       </c>
       <c r="Q33" s="1" t="str">
@@ -9742,7 +9752,7 @@
     </row>
     <row r="34" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="str">
-        <f t="shared" ref="A34:P50" si="11">_xlfn.CONCAT("[",ROW(A34)-1,",",COLUMN(A34)-1,"]")</f>
+        <f t="shared" ref="A34:P49" si="11">_xlfn.CONCAT("[",ROW(A34)-1,",",COLUMN(A34)-1,"]")</f>
         <v>[33,0]</v>
       </c>
       <c r="B34" s="1" t="str">
@@ -12552,7 +12562,7 @@
         <v>[46,45]</v>
       </c>
       <c r="AU47" s="1" t="str">
-        <f t="shared" ref="AU47:AX50" si="12">_xlfn.CONCAT("[",ROW(AU47)-1,",",COLUMN(AU47)-1,"]")</f>
+        <f t="shared" ref="AU47:AX49" si="12">_xlfn.CONCAT("[",ROW(AU47)-1,",",COLUMN(AU47)-1,"]")</f>
         <v>[46,46]</v>
       </c>
       <c r="AV47" s="1" t="str">
@@ -12694,7 +12704,7 @@
         <v>[47,30]</v>
       </c>
       <c r="AF48" s="1" t="str">
-        <f t="shared" ref="AF48:AU50" si="13">_xlfn.CONCAT("[",ROW(AF48)-1,",",COLUMN(AF48)-1,"]")</f>
+        <f t="shared" ref="AF48:AU49" si="13">_xlfn.CONCAT("[",ROW(AF48)-1,",",COLUMN(AF48)-1,"]")</f>
         <v>[47,31]</v>
       </c>
       <c r="AG48" s="5" t="str">
@@ -12832,7 +12842,7 @@
         <v>[48,14]</v>
       </c>
       <c r="P49" s="1" t="str">
-        <f t="shared" ref="P49:AE50" si="14">_xlfn.CONCAT("[",ROW(P49)-1,",",COLUMN(P49)-1,"]")</f>
+        <f t="shared" ref="P49:AE49" si="14">_xlfn.CONCAT("[",ROW(P49)-1,",",COLUMN(P49)-1,"]")</f>
         <v>[48,15]</v>
       </c>
       <c r="Q49" s="1" t="str">

</xml_diff>